<commit_message>
test pcb hoạt động adc+mpu+bitsw+button
</commit_message>
<xml_diff>
--- a/schematic/production/bom.xlsx
+++ b/schematic/production/bom.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\micromouse2024\AML_Micromouse_24_2_code\schematic\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA8F53E-DF82-4DFD-B398-EADDD0B8282B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4F7499-5FA3-45A7-948F-560565666CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D3D605D8-8968-4C55-AED7-9F4ADE23DF0C}"/>
+    <workbookView xWindow="-23148" yWindow="5412" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D3D605D8-8968-4C55-AED7-9F4ADE23DF0C}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
+    <sheet name="lên đơn" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="147">
   <si>
     <t>Designator</t>
   </si>
@@ -428,13 +442,46 @@
   </si>
   <si>
     <t>2 dây</t>
+  </si>
+  <si>
+    <t>sll</t>
+  </si>
+  <si>
+    <t>đon giá</t>
+  </si>
+  <si>
+    <t>thành giá</t>
+  </si>
+  <si>
+    <t>đơn vị</t>
+  </si>
+  <si>
+    <t>dây</t>
+  </si>
+  <si>
+    <t>cái</t>
+  </si>
+  <si>
+    <t>túi</t>
+  </si>
+  <si>
+    <t>mỗi thứ 1 túi</t>
+  </si>
+  <si>
+    <t>G020804</t>
+  </si>
+  <si>
+    <t>CLA2435</t>
+  </si>
+  <si>
+    <t>A051011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,6 +618,26 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -917,9 +984,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1297,17 +1368,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13015EB-2B70-4D74-82C7-1B1EC7497485}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="26.109375" customWidth="1"/>
-    <col min="15" max="15" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="15" max="15" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1492,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1446,7 +1518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1472,7 +1544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1498,7 +1570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1524,7 +1596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1550,7 +1622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1576,7 +1648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1602,7 +1674,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1628,7 +1700,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1654,7 +1726,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1680,7 +1752,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1706,7 +1778,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1732,7 +1804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1758,7 +1830,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1784,7 +1856,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1810,7 +1882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1836,7 +1908,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1862,7 +1934,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1888,7 +1960,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1914,7 +1986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -1940,7 +2012,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -1966,7 +2038,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -1992,7 +2064,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2018,7 +2090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -2044,7 +2116,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>93</v>
       </c>
@@ -2070,7 +2142,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -2096,7 +2168,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -2122,7 +2194,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -2148,7 +2220,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -2174,7 +2246,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>111</v>
       </c>
@@ -2194,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -2220,7 +2292,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -2240,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -2266,7 +2338,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -2292,7 +2364,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>128</v>
       </c>
@@ -2312,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>132</v>
       </c>
@@ -2333,4 +2405,1077 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA202A9-164A-4AC7-9490-D59B1CC6B0EC}">
+  <dimension ref="G11:O58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>137</v>
+      </c>
+      <c r="N11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="7:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12">
+        <v>2000</v>
+      </c>
+      <c r="N12">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="13" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>3000</v>
+      </c>
+      <c r="N13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <v>4000</v>
+      </c>
+      <c r="N14">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>2000</v>
+      </c>
+      <c r="N15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16">
+        <v>2000</v>
+      </c>
+      <c r="N16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2">
+        <f>IF(J17&gt;10,2,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>2000</v>
+      </c>
+      <c r="N17">
+        <f>M17*H17</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18:H49" si="0">IF(J18&gt;10,2,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18">
+        <v>3000</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ref="N18:N57" si="1">M18*H18</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19">
+        <v>2000</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2">
+        <v>6</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20">
+        <v>2000</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2">
+        <v>5</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21">
+        <v>3</v>
+      </c>
+      <c r="K21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21">
+        <v>1400</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22">
+        <v>2000</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23">
+        <v>1500</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>13</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24">
+        <v>2500</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="25" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>14</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25">
+        <v>3000</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="O25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="M26">
+        <v>2500</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+      <c r="O26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>16</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27">
+        <v>4500</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="O27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>17</v>
+      </c>
+      <c r="H28" s="2">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28">
+        <v>1500</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="29" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29">
+        <v>6000</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="30" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>19</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30" t="s">
+        <v>67</v>
+      </c>
+      <c r="M30">
+        <v>4500</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="O30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>20</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>134</v>
+      </c>
+      <c r="M31">
+        <v>12000</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+      <c r="K32" t="s">
+        <v>74</v>
+      </c>
+      <c r="M32">
+        <v>2000</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="33" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>22</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33" t="s">
+        <v>77</v>
+      </c>
+      <c r="M33">
+        <v>2000</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="34" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>23</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34" t="s">
+        <v>80</v>
+      </c>
+      <c r="M34">
+        <v>2000</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>24</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M35">
+        <v>3000</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="36" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>25</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>86</v>
+      </c>
+      <c r="M36">
+        <v>1800</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="37" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>26</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>89</v>
+      </c>
+      <c r="M37">
+        <v>2300</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>27</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
+      </c>
+      <c r="K38" t="s">
+        <v>92</v>
+      </c>
+      <c r="M38">
+        <v>2000</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="39" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>28</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
+        <v>95</v>
+      </c>
+      <c r="M39">
+        <v>3000</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="40" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>29</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40" t="s">
+        <v>98</v>
+      </c>
+      <c r="M40">
+        <v>3000</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>30</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41" t="s">
+        <v>102</v>
+      </c>
+      <c r="M41">
+        <v>5000</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="42" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>31</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42" t="s">
+        <v>106</v>
+      </c>
+      <c r="M42">
+        <v>4000</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="43" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>32</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="L43" t="s">
+        <v>110</v>
+      </c>
+      <c r="M43">
+        <v>7000</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="44" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>33</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>34</v>
+      </c>
+      <c r="H45" s="2">
+        <v>5</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45" t="s">
+        <v>117</v>
+      </c>
+      <c r="M45">
+        <v>1400</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="46" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>35</v>
+      </c>
+      <c r="H46" s="2">
+        <v>3</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M46">
+        <v>30000</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="47" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>36</v>
+      </c>
+      <c r="H47" s="2">
+        <v>2</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="L47" t="s">
+        <v>124</v>
+      </c>
+      <c r="M47">
+        <v>10500</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="48" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>37</v>
+      </c>
+      <c r="H48" s="2">
+        <v>5</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>127</v>
+      </c>
+      <c r="M48">
+        <v>1400</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="49" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>38</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>39</v>
+      </c>
+      <c r="H50" s="2">
+        <v>3</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M50">
+        <v>1000</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="51" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>40</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="M51">
+        <v>3000</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="52" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>41</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="M52">
+        <v>1800</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="53" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <f>SUM(N12:N57)</f>
+        <v>288400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>